<commit_message>
Add import peserta from sertifikat & minor updates
</commit_message>
<xml_diff>
--- a/public/template_peserta.xlsx
+++ b/public/template_peserta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sertifikat\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C456F1AC-9857-45B9-9C66-7952812B8F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E0F34D-FC70-460E-AFEC-36F5EC24301D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{DA67EDAA-8DD2-4F33-87AD-51F3D54E3E61}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>nik</t>
   </si>
@@ -46,27 +46,6 @@
   </si>
   <si>
     <t>jabatan</t>
-  </si>
-  <si>
-    <t>3578200408990002</t>
-  </si>
-  <si>
-    <t>Joko</t>
-  </si>
-  <si>
-    <t>Sby</t>
-  </si>
-  <si>
-    <t>2020-01-01</t>
-  </si>
-  <si>
-    <t>Jalan</t>
-  </si>
-  <si>
-    <t>Dinas Kes</t>
-  </si>
-  <si>
-    <t>Staf</t>
   </si>
 </sst>
 </file>
@@ -419,15 +398,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48BCCEBF-4A3B-4000-A615-1AA09C172579}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="9.140625" style="1"/>
+    <col min="1" max="1" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -453,29 +433,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>